<commit_message>
Updated to include column for incidence rate
</commit_message>
<xml_diff>
--- a/2017/datacall/OWASP Top 10 - 2017 Data Call-Public Template.xlsx
+++ b/2017/datacall/OWASP Top 10 - 2017 Data Call-Public Template.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28702"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Brian/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Brian/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Name of Company/Organization</t>
   </si>
@@ -185,6 +185,12 @@
     <t>You can find the answer options for questions 10-17 on the 
 OWASP Wiki: https://www.owasp.org/index.php/Category:OWASP_Top_Ten_Project#tab=OWASP_Top_10_for_2017_Release_Candidate
 Or on the Google Form: https://docs.google.com/forms/d/1sBMHN5nBicjr5xSo04xkdP5JlCnXFcKFCgEHjwPGuLw/edit</t>
+  </si>
+  <si>
+    <t>Number of Unique Applications with this CWE</t>
+  </si>
+  <si>
+    <t>Total number of CWEs found</t>
   </si>
 </sst>
 </file>
@@ -220,6 +226,7 @@
       <sz val="20"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -236,7 +243,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -336,6 +343,57 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -358,7 +416,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -370,13 +428,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -388,11 +439,63 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -751,110 +854,124 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P55"/>
+  <dimension ref="A1:Q57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="75.33203125" customWidth="1"/>
-    <col min="2" max="2" width="64.1640625" customWidth="1"/>
-    <col min="3" max="12" width="8.83203125" style="2"/>
-    <col min="13" max="14" width="9.1640625" style="2" customWidth="1"/>
-    <col min="15" max="16" width="8.83203125" style="2"/>
+    <col min="2" max="2" width="40" customWidth="1"/>
+    <col min="3" max="3" width="36.83203125" customWidth="1"/>
+    <col min="4" max="13" width="8.83203125" style="2"/>
+    <col min="14" max="15" width="9.1640625" style="2" customWidth="1"/>
+    <col min="16" max="17" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:16" ht="26" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+    <row r="1" spans="1:17" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:17" ht="26" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="M2" s="3"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="15"/>
       <c r="N2" s="3"/>
-    </row>
-    <row r="3" spans="1:16" ht="52" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="17" t="s">
+      <c r="O2" s="3"/>
+    </row>
+    <row r="3" spans="1:17" ht="52" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="M3" s="3"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="17"/>
       <c r="N3" s="3"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A4" s="10" t="s">
+      <c r="O3" s="3"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="6"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A5" s="10" t="s">
+      <c r="B4" s="25"/>
+      <c r="C4" s="26"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="6"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A6" s="10" t="s">
+      <c r="B5" s="23"/>
+      <c r="C5" s="24"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="6"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A7" s="10" t="s">
+      <c r="B6" s="23"/>
+      <c r="C6" s="24"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A7" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="6"/>
-    </row>
-    <row r="8" spans="1:16" ht="26" x14ac:dyDescent="0.15">
-      <c r="A8" s="11" t="s">
+      <c r="B7" s="23"/>
+      <c r="C7" s="24"/>
+    </row>
+    <row r="8" spans="1:17" ht="26" x14ac:dyDescent="0.15">
+      <c r="A8" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="6"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A9" s="10" t="s">
+      <c r="B8" s="27"/>
+      <c r="C8" s="28"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A9" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="6"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A10" s="10" t="s">
+      <c r="B9" s="23"/>
+      <c r="C9" s="24"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="6"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A11" s="10" t="s">
+      <c r="B10" s="23"/>
+      <c r="C10" s="24"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="6"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A12" s="10" t="s">
+      <c r="B11" s="23"/>
+      <c r="C11" s="24"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A12" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="6"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A13" s="10" t="s">
+      <c r="B12" s="23"/>
+      <c r="C12" s="24"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A13" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="6"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A14" s="10" t="s">
+      <c r="B13" s="23"/>
+      <c r="C13" s="24"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A14" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="6"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A15" s="10" t="s">
+      <c r="B14" s="23"/>
+      <c r="C14" s="24"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A15" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="4"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="24"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
@@ -866,13 +983,14 @@
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A16" s="10" t="s">
+      <c r="O15" s="4"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A16" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="3"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="24"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -884,273 +1002,349 @@
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="5"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A17" s="10" t="s">
+      <c r="O16" s="3"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="5"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A17" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="O17" s="4"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A18" s="12" t="s">
+      <c r="B17" s="23"/>
+      <c r="C17" s="24"/>
+      <c r="P17" s="4"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A18" s="7"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="24"/>
+      <c r="P18" s="4"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A19" s="7"/>
+      <c r="B19" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="P19" s="4"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A20" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="O18" s="4"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A19" s="12" t="s">
+      <c r="B20" s="30"/>
+      <c r="C20" s="31"/>
+      <c r="P20" s="4"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A21" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="O19" s="4"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A20" s="12" t="s">
+      <c r="B21" s="30"/>
+      <c r="C21" s="31"/>
+      <c r="P21" s="4"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A22" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="O20" s="4"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A21" s="12" t="s">
+      <c r="B22" s="30"/>
+      <c r="C22" s="31"/>
+      <c r="P22" s="4"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A23" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="O21" s="4"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A22" s="12" t="s">
+      <c r="B23" s="30"/>
+      <c r="C23" s="31"/>
+      <c r="P23" s="4"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A24" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="O22" s="4"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A23" s="12" t="s">
+      <c r="B24" s="30"/>
+      <c r="C24" s="31"/>
+      <c r="P24" s="4"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A25" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="O23" s="4"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A24" s="12" t="s">
+      <c r="B25" s="30"/>
+      <c r="C25" s="31"/>
+      <c r="P25" s="4"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A26" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="O24" s="4"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A25" s="12" t="s">
+      <c r="B26" s="30"/>
+      <c r="C26" s="31"/>
+      <c r="P26" s="4"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A27" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="6"/>
-      <c r="O25" s="4"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A26" s="12" t="s">
+      <c r="B27" s="30"/>
+      <c r="C27" s="31"/>
+      <c r="P27" s="4"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A28" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="6"/>
-      <c r="O26" s="4"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A27" s="12" t="s">
+      <c r="B28" s="30"/>
+      <c r="C28" s="31"/>
+      <c r="P28" s="4"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A29" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="6"/>
-      <c r="O27" s="4"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A28" s="12" t="s">
+      <c r="B29" s="30"/>
+      <c r="C29" s="31"/>
+      <c r="P29" s="4"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A30" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="6"/>
-      <c r="O28" s="4"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A29" s="12" t="s">
+      <c r="B30" s="30"/>
+      <c r="C30" s="31"/>
+      <c r="P30" s="4"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A31" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="O29" s="4"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A30" s="12" t="s">
+      <c r="B31" s="30"/>
+      <c r="C31" s="31"/>
+      <c r="P31" s="4"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A32" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B30" s="6"/>
-      <c r="O30" s="4"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A31" s="12" t="s">
+      <c r="B32" s="30"/>
+      <c r="C32" s="31"/>
+      <c r="P32" s="4"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A33" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="6"/>
-      <c r="O31" s="4"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A32" s="12" t="s">
+      <c r="B33" s="30"/>
+      <c r="C33" s="31"/>
+      <c r="P33" s="4"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A34" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B32" s="6"/>
-      <c r="O32" s="4"/>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A33" s="12" t="s">
+      <c r="B34" s="30"/>
+      <c r="C34" s="31"/>
+      <c r="P34" s="4"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A35" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B33" s="6"/>
-      <c r="O33" s="4"/>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A34" s="12" t="s">
+      <c r="B35" s="30"/>
+      <c r="C35" s="31"/>
+      <c r="P35" s="4"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A36" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B34" s="6"/>
-      <c r="O34" s="4"/>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A35" s="12" t="s">
+      <c r="B36" s="30"/>
+      <c r="C36" s="31"/>
+      <c r="P36" s="4"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A37" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B35" s="6"/>
-      <c r="O35" s="4"/>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A36" s="12" t="s">
+      <c r="B37" s="30"/>
+      <c r="C37" s="31"/>
+      <c r="P37" s="4"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A38" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B36" s="6"/>
-      <c r="O36" s="4"/>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A37" s="12" t="s">
+      <c r="B38" s="30"/>
+      <c r="C38" s="31"/>
+      <c r="P38" s="4"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A39" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B37" s="6"/>
-      <c r="O37" s="4"/>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A38" s="12" t="s">
+      <c r="B39" s="30"/>
+      <c r="C39" s="31"/>
+      <c r="P39" s="4"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A40" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B38" s="6"/>
-      <c r="O38" s="4"/>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A39" s="12" t="s">
+      <c r="B40" s="30"/>
+      <c r="C40" s="31"/>
+      <c r="P40" s="4"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A41" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B39" s="6"/>
-      <c r="O39" s="4"/>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A40" s="12" t="s">
+      <c r="B41" s="30"/>
+      <c r="C41" s="31"/>
+      <c r="P41" s="4"/>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A42" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B40" s="6"/>
-      <c r="O40" s="4"/>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A41" s="12" t="s">
+      <c r="B42" s="30"/>
+      <c r="C42" s="31"/>
+      <c r="P42" s="4"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A43" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B41" s="6"/>
-      <c r="O41" s="4"/>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A42" s="12" t="s">
+      <c r="B43" s="30"/>
+      <c r="C43" s="31"/>
+      <c r="P43" s="4"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A44" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B42" s="6"/>
-      <c r="O42" s="4"/>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A43" s="12" t="s">
+      <c r="B44" s="30"/>
+      <c r="C44" s="31"/>
+      <c r="P44" s="4"/>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A45" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B43" s="6"/>
-      <c r="O43" s="4"/>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A44" s="12" t="s">
+      <c r="B45" s="30"/>
+      <c r="C45" s="31"/>
+      <c r="P45" s="4"/>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A46" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B44" s="6"/>
-      <c r="O44" s="4"/>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A45" s="12" t="s">
+      <c r="B46" s="30"/>
+      <c r="C46" s="31"/>
+      <c r="P46" s="4"/>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A47" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B45" s="6"/>
-      <c r="O45" s="4"/>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A46" s="12" t="s">
+      <c r="B47" s="30"/>
+      <c r="C47" s="31"/>
+      <c r="P47" s="4"/>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A48" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B46" s="6"/>
-      <c r="O46" s="4"/>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A47" s="12" t="s">
+      <c r="B48" s="30"/>
+      <c r="C48" s="31"/>
+      <c r="P48" s="4"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A49" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B47" s="6"/>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A48" s="13" t="s">
+      <c r="B49" s="30"/>
+      <c r="C49" s="31"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A50" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B48" s="6"/>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A49" s="14"/>
-      <c r="B49" s="6"/>
-    </row>
-    <row r="50" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="10"/>
-      <c r="B50" s="6"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A51" s="15" t="s">
+      <c r="B50" s="30"/>
+      <c r="C50" s="31"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A51" s="11"/>
+      <c r="B51" s="21"/>
+      <c r="C51" s="6"/>
+    </row>
+    <row r="52" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A52" s="7"/>
+      <c r="B52" s="20"/>
+      <c r="C52" s="6"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A53" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B51" s="6"/>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A52" s="15" t="s">
+      <c r="B53" s="23"/>
+      <c r="C53" s="24"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A54" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B52" s="6"/>
-    </row>
-    <row r="53" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="15" t="s">
+      <c r="B54" s="23"/>
+      <c r="C54" s="24"/>
+    </row>
+    <row r="55" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A55" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B53" s="6"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A54" s="15" t="s">
+      <c r="B55" s="23"/>
+      <c r="C55" s="24"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A56" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B54" s="6"/>
-    </row>
-    <row r="55" spans="1:2" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="16" t="s">
+      <c r="B56" s="23"/>
+      <c r="C56" s="24"/>
+    </row>
+    <row r="57" spans="1:3" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B55" s="7"/>
+      <c r="B57" s="32"/>
+      <c r="C57" s="33"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
+  <mergeCells count="22">
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B4:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>